<commit_message>
till sprint backlog 3
</commit_message>
<xml_diff>
--- a/Product Backlog Titans.xlsx
+++ b/Product Backlog Titans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\College Things\Projects\titans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\College Things\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E8CE2E12-4086-4DA4-968C-34E590A5C3DA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7D3DF830-43A8-4352-8CEC-F8EA85D3CEC5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" tabRatio="936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" tabRatio="936" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="340">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -1051,10 +1051,10 @@
     <t>IN PROGRESS</t>
   </si>
   <si>
-    <t>NOT STARTED</t>
-  </si>
-  <si>
     <t>NOT COMPLETED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse the content of the person I want to follow  </t>
   </si>
 </sst>
 </file>
@@ -1488,10 +1488,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1500,19 +1513,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1522,12 +1532,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1535,6 +1539,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1599,13 +1606,6 @@
     </xf>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3584,7 +3584,7 @@
   </sheetPr>
   <dimension ref="A3:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -3602,17 +3602,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D4" s="32" t="s">
@@ -3621,33 +3621,33 @@
       <c r="E4" s="33"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46" t="s">
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="49" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
@@ -3657,10 +3657,10 @@
       <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="13"/>
-      <c r="H7" s="85">
+      <c r="H7" s="47">
         <v>43347</v>
       </c>
       <c r="I7" s="13"/>
@@ -3707,7 +3707,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="13"/>
-      <c r="H8" s="85">
+      <c r="H8" s="47">
         <v>43347</v>
       </c>
       <c r="I8" s="13"/>
@@ -3732,7 +3732,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="13"/>
-      <c r="H9" s="85">
+      <c r="H9" s="47">
         <v>43347</v>
       </c>
       <c r="I9" s="13"/>
@@ -3757,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="13"/>
-      <c r="H10" s="85">
+      <c r="H10" s="47">
         <v>43347</v>
       </c>
       <c r="I10" s="13"/>
@@ -3782,7 +3782,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="13"/>
-      <c r="H11" s="85">
+      <c r="H11" s="47">
         <v>43347</v>
       </c>
       <c r="I11" s="13"/>
@@ -3807,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="13"/>
-      <c r="H12" s="85">
+      <c r="H12" s="47">
         <v>43354</v>
       </c>
       <c r="I12" s="13"/>
@@ -3832,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="13"/>
-      <c r="H13" s="85">
+      <c r="H13" s="47">
         <v>43355</v>
       </c>
       <c r="I13" s="13"/>
@@ -3857,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="13"/>
-      <c r="H14" s="85">
+      <c r="H14" s="47">
         <v>43357</v>
       </c>
       <c r="I14" s="13"/>
@@ -3882,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="13"/>
-      <c r="H15" s="85">
+      <c r="H15" s="47">
         <v>43357</v>
       </c>
       <c r="I15" s="13"/>
@@ -3905,7 +3905,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="13"/>
-      <c r="H16" s="85">
+      <c r="H16" s="47">
         <v>43359</v>
       </c>
       <c r="I16" s="13"/>
@@ -3930,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="85">
+      <c r="H17" s="47">
         <v>43359</v>
       </c>
       <c r="I17" s="13"/>
@@ -3955,7 +3955,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="85">
+      <c r="H18" s="47">
         <v>43361</v>
       </c>
       <c r="I18" s="13"/>
@@ -3980,7 +3980,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="85">
+      <c r="H19" s="47">
         <v>43368</v>
       </c>
       <c r="I19" s="13"/>
@@ -4005,7 +4005,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="13"/>
-      <c r="H20" s="85">
+      <c r="H20" s="47">
         <v>43368</v>
       </c>
       <c r="I20" s="13"/>
@@ -4030,7 +4030,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="13"/>
-      <c r="H21" s="85">
+      <c r="H21" s="47">
         <v>43371</v>
       </c>
       <c r="I21" s="13"/>
@@ -4055,7 +4055,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="13"/>
-      <c r="H22" s="85">
+      <c r="H22" s="47">
         <v>43375</v>
       </c>
       <c r="I22" s="13"/>
@@ -4080,7 +4080,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="13"/>
-      <c r="H23" s="85">
+      <c r="H23" s="47">
         <v>43375</v>
       </c>
       <c r="I23" s="13"/>
@@ -4105,7 +4105,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="13"/>
-      <c r="H24" s="85">
+      <c r="H24" s="47">
         <v>43378</v>
       </c>
       <c r="I24" s="13"/>
@@ -4130,7 +4130,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="13"/>
-      <c r="H25" s="85">
+      <c r="H25" s="47">
         <v>43378</v>
       </c>
       <c r="I25" s="13"/>
@@ -4155,7 +4155,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="13"/>
-      <c r="H26" s="85">
+      <c r="H26" s="47">
         <v>43380</v>
       </c>
       <c r="I26" s="13"/>
@@ -4180,7 +4180,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="13"/>
-      <c r="H27" s="85">
+      <c r="H27" s="47">
         <v>43382</v>
       </c>
       <c r="I27" s="13"/>
@@ -4205,7 +4205,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="85">
+      <c r="H28" s="47">
         <v>43389</v>
       </c>
       <c r="I28" s="13"/>
@@ -4230,7 +4230,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="85">
+      <c r="H29" s="47">
         <v>43391</v>
       </c>
       <c r="I29" s="13"/>
@@ -4253,7 +4253,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="13"/>
-      <c r="H30" s="85">
+      <c r="H30" s="47">
         <v>43391</v>
       </c>
       <c r="I30" s="13"/>
@@ -4278,7 +4278,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="85">
+      <c r="H31" s="47">
         <v>43393</v>
       </c>
       <c r="I31" s="13"/>
@@ -4303,7 +4303,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="13"/>
-      <c r="H32" s="85">
+      <c r="H32" s="47">
         <v>43394</v>
       </c>
       <c r="I32" s="13"/>
@@ -4328,7 +4328,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="85">
+      <c r="H33" s="47">
         <v>43395</v>
       </c>
       <c r="I33" s="13"/>
@@ -4353,7 +4353,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="13"/>
-      <c r="H34" s="85">
+      <c r="H34" s="47">
         <v>43396</v>
       </c>
       <c r="I34" s="13"/>
@@ -4378,7 +4378,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="85">
+      <c r="H35" s="47">
         <v>43475</v>
       </c>
       <c r="I35" s="13"/>
@@ -4403,7 +4403,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="85">
+      <c r="H36" s="47">
         <v>43476</v>
       </c>
       <c r="I36" s="13"/>
@@ -4428,7 +4428,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="13"/>
-      <c r="H37" s="85">
+      <c r="H37" s="47">
         <v>43477</v>
       </c>
       <c r="I37" s="13"/>
@@ -4453,7 +4453,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="85">
+      <c r="H38" s="47">
         <v>43478</v>
       </c>
       <c r="I38" s="13"/>
@@ -4478,7 +4478,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="85">
+      <c r="H39" s="47">
         <v>43479</v>
       </c>
       <c r="I39" s="13"/>
@@ -4503,7 +4503,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="85">
+      <c r="H40" s="47">
         <v>43480</v>
       </c>
       <c r="I40" s="13"/>
@@ -6302,11 +6302,11 @@
       <c r="A4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
@@ -6332,10 +6332,10 @@
       <c r="C8" s="42">
         <v>19</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="73"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
@@ -6347,8 +6347,8 @@
       <c r="C9" s="42">
         <v>19</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
@@ -6360,8 +6360,8 @@
       <c r="C10" s="42">
         <v>19</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
@@ -6373,8 +6373,8 @@
       <c r="C11" s="42">
         <v>19</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
@@ -6386,8 +6386,8 @@
       <c r="C12" s="42">
         <v>19</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
@@ -6399,42 +6399,42 @@
       <c r="C13" s="42">
         <v>19</v>
       </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
+      <c r="A14" s="45"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
-      <c r="I20" s="74" t="s">
+      <c r="I20" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
@@ -6483,15 +6483,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6526,21 +6526,21 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="59" t="s">
         <v>333</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="53">
+      <c r="A6" s="55">
         <v>1</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="80" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -6553,15 +6553,15 @@
         <v>225</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G6" s="26">
         <v>43475</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="78"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="34" t="s">
         <v>314</v>
       </c>
@@ -6572,15 +6572,15 @@
         <v>226</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G7" s="26">
         <v>43475</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
-      <c r="B8" s="79"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="34" t="s">
         <v>315</v>
       </c>
@@ -6591,17 +6591,17 @@
         <v>227</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G8" s="26">
         <v>43475</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="53">
+      <c r="A9" s="55">
         <v>2</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="60" t="s">
         <v>118</v>
       </c>
       <c r="C9" s="34" t="s">
@@ -6614,15 +6614,15 @@
         <v>225</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G9" s="26">
         <v>43476</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="34" t="s">
         <v>317</v>
       </c>
@@ -6633,15 +6633,15 @@
         <v>226</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G10" s="26">
         <v>43476</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="34" t="s">
         <v>318</v>
       </c>
@@ -6652,17 +6652,17 @@
         <v>227</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G11" s="26">
         <v>43476</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="53">
+      <c r="A12" s="55">
         <v>3</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="34" t="s">
@@ -6675,15 +6675,15 @@
         <v>225</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G12" s="26">
         <v>43477</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
-      <c r="B13" s="48"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="34" t="s">
         <v>320</v>
       </c>
@@ -6694,15 +6694,15 @@
         <v>226</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G13" s="26">
         <v>43477</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="34" t="s">
         <v>321</v>
       </c>
@@ -6713,17 +6713,17 @@
         <v>227</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G14" s="26">
         <v>43477</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="53">
+      <c r="A15" s="55">
         <v>4</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="60" t="s">
         <v>306</v>
       </c>
       <c r="C15" s="34" t="s">
@@ -6736,15 +6736,15 @@
         <v>225</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G15" s="26">
         <v>43478</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="53"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="34" t="s">
         <v>323</v>
       </c>
@@ -6755,15 +6755,15 @@
         <v>226</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G16" s="26">
         <v>43478</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="34" t="s">
         <v>324</v>
       </c>
@@ -6774,17 +6774,17 @@
         <v>227</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G17" s="26">
         <v>43478</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53">
+      <c r="A18" s="55">
         <v>5</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="52" t="s">
         <v>128</v>
       </c>
       <c r="C18" s="34" t="s">
@@ -6797,15 +6797,15 @@
         <v>227</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G18" s="26">
         <v>43478</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="53"/>
-      <c r="B19" s="48"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="34" t="s">
         <v>326</v>
       </c>
@@ -6816,15 +6816,15 @@
         <v>226</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G19" s="26">
         <v>43479</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="53"/>
-      <c r="B20" s="48"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="34" t="s">
         <v>327</v>
       </c>
@@ -6835,17 +6835,17 @@
         <v>225</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G20" s="26">
         <v>43479</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="53">
+      <c r="A21" s="55">
         <v>6</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="83" t="s">
         <v>165</v>
       </c>
       <c r="C21" s="34" t="s">
@@ -6858,15 +6858,15 @@
         <v>198</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G21" s="26">
         <v>43479</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
-      <c r="B22" s="80"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="34" t="s">
         <v>329</v>
       </c>
@@ -6877,15 +6877,15 @@
         <v>225</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G22" s="26">
         <v>43480</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="34" t="s">
         <v>330</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>312</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G23" s="26">
         <v>43480</v>
@@ -6949,51 +6949,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -7011,16 +7011,16 @@
       <c r="E4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="71"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="74"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
@@ -7040,27 +7040,27 @@
       <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="77">
+      <c r="A7" s="80">
         <v>1</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="80" t="s">
         <v>114</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -7080,8 +7080,8 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="10" t="s">
         <v>286</v>
       </c>
@@ -7099,8 +7099,8 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="43" t="s">
         <v>285</v>
       </c>
@@ -7118,10 +7118,10 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="58">
+      <c r="A10" s="60">
         <v>2</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="60" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -7141,8 +7141,8 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="10" t="s">
         <v>286</v>
       </c>
@@ -7160,8 +7160,8 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="44" t="s">
         <v>285</v>
       </c>
@@ -7179,10 +7179,10 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="47">
+      <c r="A13" s="52">
         <v>3</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -7202,8 +7202,8 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="10" t="s">
         <v>286</v>
       </c>
@@ -7221,8 +7221,8 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="43" t="s">
         <v>285</v>
       </c>
@@ -7240,10 +7240,10 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="58">
+      <c r="A16" s="60">
         <v>4</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="60" t="s">
         <v>306</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -7263,8 +7263,8 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="10" t="s">
         <v>286</v>
       </c>
@@ -7282,8 +7282,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="43" t="s">
         <v>285</v>
       </c>
@@ -7301,10 +7301,10 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="47">
+      <c r="A19" s="52">
         <v>5</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="52" t="s">
         <v>128</v>
       </c>
       <c r="C19" s="44" t="s">
@@ -7324,8 +7324,8 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="8" t="s">
         <v>307</v>
       </c>
@@ -7343,8 +7343,8 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="10" t="s">
         <v>308</v>
       </c>
@@ -7362,10 +7362,10 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="80">
+      <c r="A22" s="83">
         <v>6</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="83" t="s">
         <v>165</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -7385,8 +7385,8 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="6" t="s">
         <v>310</v>
       </c>
@@ -7404,8 +7404,8 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="6" t="s">
         <v>311</v>
       </c>
@@ -7552,10 +7552,10 @@
       <c r="C8" s="42">
         <v>18</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="73"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
@@ -7567,8 +7567,8 @@
       <c r="C9" s="42">
         <v>18</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
@@ -7580,8 +7580,8 @@
       <c r="C10" s="42">
         <v>18</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
@@ -7593,8 +7593,8 @@
       <c r="C11" s="42">
         <v>18</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
@@ -7606,8 +7606,8 @@
       <c r="C12" s="42">
         <v>18</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
@@ -7619,42 +7619,42 @@
       <c r="C13" s="42">
         <v>18</v>
       </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
+      <c r="A14" s="45"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
-      <c r="I20" s="74" t="s">
+      <c r="I20" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
@@ -7686,7 +7686,7 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -7703,15 +7703,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -7746,21 +7746,21 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="60" t="s">
         <v>130</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -7781,7 +7781,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="57"/>
-      <c r="B7" s="59"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
@@ -7797,11 +7797,11 @@
       <c r="G7" s="26">
         <v>43347</v>
       </c>
-      <c r="I7" s="83"/>
+      <c r="I7" s="45"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="57"/>
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="7" t="s">
         <v>30</v>
       </c>
@@ -7817,11 +7817,11 @@
       <c r="G8" s="26">
         <v>43347</v>
       </c>
-      <c r="I8" s="83"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="57"/>
-      <c r="B9" s="59"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
@@ -7837,13 +7837,13 @@
       <c r="G9" s="26">
         <v>43347</v>
       </c>
-      <c r="I9" s="83"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="52" t="s">
         <v>132</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -7861,11 +7861,11 @@
       <c r="G10" s="26">
         <v>43347</v>
       </c>
-      <c r="I10" s="83"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="57"/>
-      <c r="B11" s="48"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="7" t="s">
         <v>33</v>
       </c>
@@ -7881,11 +7881,11 @@
       <c r="G11" s="26">
         <v>43347</v>
       </c>
-      <c r="I11" s="83"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="57"/>
-      <c r="B12" s="48"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="7" t="s">
         <v>34</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="G12" s="26">
         <v>43347</v>
       </c>
-      <c r="I12" s="83"/>
+      <c r="I12" s="45"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56" t="s">
@@ -7973,7 +7973,7 @@
       <c r="A16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="52" t="s">
         <v>137</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -7994,7 +7994,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="57"/>
-      <c r="B17" s="48"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="7" t="s">
         <v>39</v>
       </c>
@@ -8038,7 +8038,7 @@
       <c r="A19" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="52" t="s">
         <v>141</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -8059,7 +8059,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="57"/>
-      <c r="B20" s="48"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="57"/>
-      <c r="B21" s="48"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="7" t="s">
         <v>43</v>
       </c>
@@ -8096,8 +8096,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="60"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="7" t="s">
         <v>44</v>
       </c>
@@ -8203,10 +8203,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="52" t="s">
         <v>147</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -8226,8 +8226,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="53"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="7" t="s">
         <v>50</v>
       </c>
@@ -8245,7 +8245,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="55" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="50" t="s">
@@ -8268,7 +8268,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="53"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="51"/>
       <c r="C30" s="7" t="s">
         <v>52</v>
@@ -8287,8 +8287,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="53"/>
-      <c r="B31" s="52"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="7" t="s">
         <v>53</v>
       </c>
@@ -8319,13 +8319,13 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B31"/>
@@ -8358,51 +8358,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -8420,16 +8420,16 @@
       <c r="E4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="71"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="74"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
@@ -8449,27 +8449,27 @@
       <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="59">
+      <c r="A7" s="61">
         <v>1</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="61" t="s">
         <v>130</v>
       </c>
       <c r="C7" s="41" t="s">
@@ -8489,8 +8489,8 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="6" t="s">
         <v>199</v>
       </c>
@@ -8508,8 +8508,8 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="6" t="s">
         <v>200</v>
       </c>
@@ -8527,8 +8527,8 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="6" t="s">
         <v>201</v>
       </c>
@@ -8546,10 +8546,10 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="47">
+      <c r="A11" s="52">
         <v>2</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="52" t="s">
         <v>132</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -8569,8 +8569,8 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="48"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="6" t="s">
         <v>212</v>
       </c>
@@ -8588,8 +8588,8 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="48"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="6" t="s">
         <v>213</v>
       </c>
@@ -8672,10 +8672,10 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="47">
+      <c r="A17" s="52">
         <v>5</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="52" t="s">
         <v>137</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -8695,8 +8695,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="11" t="s">
         <v>219</v>
       </c>
@@ -8737,10 +8737,10 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="47">
+      <c r="A20" s="52">
         <v>7</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="52" t="s">
         <v>141</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -8760,8 +8760,8 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="8" t="s">
         <v>222</v>
       </c>
@@ -8779,8 +8779,8 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="10" t="s">
         <v>223</v>
       </c>
@@ -8798,8 +8798,8 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="6" t="s">
         <v>224</v>
       </c>
@@ -8905,10 +8905,10 @@
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="47">
+      <c r="A28" s="52">
         <v>11</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="52" t="s">
         <v>147</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -8928,8 +8928,8 @@
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="48"/>
-      <c r="B29" s="48"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="8" t="s">
         <v>233</v>
       </c>
@@ -8989,8 +8989,8 @@
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="8" t="s">
         <v>236</v>
       </c>
@@ -9063,25 +9063,25 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="19">
+    <mergeCell ref="A1:M3"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A1:M3"/>
-    <mergeCell ref="F4:M4"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="94" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -9119,11 +9119,11 @@
       <c r="A4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
@@ -9149,10 +9149,10 @@
       <c r="C8" s="42">
         <v>26</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="73"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
@@ -9164,8 +9164,8 @@
       <c r="C9" s="42">
         <v>16</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
@@ -9177,8 +9177,8 @@
       <c r="C10" s="42">
         <v>16</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
@@ -9190,8 +9190,8 @@
       <c r="C11" s="42">
         <v>16</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
@@ -9203,8 +9203,8 @@
       <c r="C12" s="42">
         <v>16</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
@@ -9216,45 +9216,45 @@
       <c r="C13" s="42">
         <v>16</v>
       </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
-      <c r="I20" s="74" t="s">
+      <c r="I20" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
@@ -9300,8 +9300,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9316,15 +9316,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -9359,21 +9359,21 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="59" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="80" t="s">
         <v>149</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -9393,8 +9393,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="78"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="15" t="s">
         <v>55</v>
       </c>
@@ -9412,8 +9412,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
-      <c r="B8" s="79"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="15" t="s">
         <v>56</v>
       </c>
@@ -9431,10 +9431,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="60" t="s">
         <v>151</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -9454,8 +9454,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="15" t="s">
         <v>58</v>
       </c>
@@ -9473,8 +9473,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="15" t="s">
         <v>59</v>
       </c>
@@ -9492,10 +9492,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="52" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -9515,8 +9515,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
-      <c r="B13" s="48"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="15" t="s">
         <v>61</v>
       </c>
@@ -9534,8 +9534,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="15" t="s">
         <v>62</v>
       </c>
@@ -9553,10 +9553,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="60" t="s">
         <v>152</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -9576,8 +9576,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="53"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="15" t="s">
         <v>64</v>
       </c>
@@ -9595,8 +9595,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="15" t="s">
         <v>65</v>
       </c>
@@ -9614,10 +9614,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="52" t="s">
         <v>153</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -9637,8 +9637,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="53"/>
-      <c r="B19" s="48"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="15" t="s">
         <v>67</v>
       </c>
@@ -9656,8 +9656,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="53"/>
-      <c r="B20" s="48"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="15" t="s">
         <v>68</v>
       </c>
@@ -9675,10 +9675,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="60" t="s">
         <v>154</v>
       </c>
       <c r="C21" s="15" t="s">
@@ -9698,8 +9698,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
-      <c r="B22" s="59"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="15" t="s">
         <v>70</v>
       </c>
@@ -9717,8 +9717,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="59"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="15" t="s">
         <v>71</v>
       </c>
@@ -9736,10 +9736,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="60" t="s">
         <v>155</v>
       </c>
       <c r="C24" s="15" t="s">
@@ -9751,14 +9751,16 @@
       <c r="E24" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G24" s="26">
         <v>43378</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="53"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="15" t="s">
         <v>73</v>
       </c>
@@ -9768,14 +9770,16 @@
       <c r="E25" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G25" s="26">
         <v>43378</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="53"/>
-      <c r="B26" s="59"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="15" t="s">
         <v>74</v>
       </c>
@@ -9785,16 +9789,18 @@
       <c r="E26" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G26" s="26">
         <v>43380</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="52" t="s">
         <v>156</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -9806,14 +9812,16 @@
       <c r="E27" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G27" s="26">
         <v>43380</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="53"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="15" t="s">
         <v>76</v>
       </c>
@@ -9823,14 +9831,16 @@
       <c r="E28" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G28" s="26">
         <v>43380</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="53"/>
-      <c r="B29" s="48"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="15" t="s">
         <v>77</v>
       </c>
@@ -9840,16 +9850,18 @@
       <c r="E29" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G29" s="26">
         <v>43382</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="79" t="s">
         <v>157</v>
       </c>
       <c r="C30" s="34" t="s">
@@ -9861,14 +9873,16 @@
       <c r="E30" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F30" s="9"/>
+      <c r="F30" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G30" s="26">
         <v>43382</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="53"/>
-      <c r="B31" s="76"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="34" t="s">
         <v>76</v>
       </c>
@@ -9878,14 +9892,16 @@
       <c r="E31" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G31" s="26">
         <v>43382</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="53"/>
-      <c r="B32" s="76"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="34" t="s">
         <v>77</v>
       </c>
@@ -9895,7 +9911,9 @@
       <c r="E32" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F32" s="9"/>
+      <c r="F32" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G32" s="26">
         <v>43382</v>
       </c>
@@ -9909,6 +9927,18 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="20">
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="A15:A17"/>
@@ -9917,18 +9947,6 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -9940,7 +9958,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -9953,51 +9971,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -10015,16 +10033,16 @@
       <c r="E4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="71"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="74"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
@@ -10044,27 +10062,27 @@
       <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="81">
+      <c r="A7" s="84">
         <v>1</v>
       </c>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="84" t="s">
         <v>149</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -10084,8 +10102,8 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="81"/>
-      <c r="B8" s="81"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="8" t="s">
         <v>238</v>
       </c>
@@ -10103,8 +10121,8 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
-      <c r="B9" s="81"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="8" t="s">
         <v>239</v>
       </c>
@@ -10122,10 +10140,10 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="80">
+      <c r="A10" s="83">
         <v>2</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="83" t="s">
         <v>151</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -10145,8 +10163,8 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="8" t="s">
         <v>241</v>
       </c>
@@ -10164,8 +10182,8 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="80"/>
-      <c r="B12" s="80"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="8" t="s">
         <v>242</v>
       </c>
@@ -10183,10 +10201,10 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="76">
+      <c r="A13" s="79">
         <v>3</v>
       </c>
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="79" t="s">
         <v>169</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -10206,8 +10224,8 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="76"/>
-      <c r="B14" s="76"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="8" t="s">
         <v>244</v>
       </c>
@@ -10225,8 +10243,8 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="76"/>
-      <c r="B15" s="76"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="8" t="s">
         <v>245</v>
       </c>
@@ -10244,10 +10262,10 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="80">
+      <c r="A16" s="83">
         <v>4</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="83" t="s">
         <v>152</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -10267,8 +10285,8 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="8" t="s">
         <v>247</v>
       </c>
@@ -10286,8 +10304,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="8" t="s">
         <v>248</v>
       </c>
@@ -10305,10 +10323,10 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="76">
+      <c r="A19" s="79">
         <v>5</v>
       </c>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="79" t="s">
         <v>153</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -10328,8 +10346,8 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="79"/>
       <c r="C20" s="8" t="s">
         <v>250</v>
       </c>
@@ -10347,8 +10365,8 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="76"/>
-      <c r="B21" s="76"/>
+      <c r="A21" s="79"/>
+      <c r="B21" s="79"/>
       <c r="C21" s="8" t="s">
         <v>251</v>
       </c>
@@ -10366,10 +10384,10 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="80">
+      <c r="A22" s="83">
         <v>6</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="83" t="s">
         <v>154</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -10389,8 +10407,8 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="8" t="s">
         <v>253</v>
       </c>
@@ -10408,8 +10426,8 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="8" t="s">
         <v>254</v>
       </c>
@@ -10427,10 +10445,10 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="80">
+      <c r="A25" s="83">
         <v>7</v>
       </c>
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="83" t="s">
         <v>155</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -10450,8 +10468,8 @@
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="83"/>
       <c r="C26" s="8" t="s">
         <v>262</v>
       </c>
@@ -10469,8 +10487,8 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="80"/>
-      <c r="B27" s="80"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="8" t="s">
         <v>263</v>
       </c>
@@ -10488,10 +10506,10 @@
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="76">
+      <c r="A28" s="79">
         <v>8</v>
       </c>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="79" t="s">
         <v>156</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -10511,8 +10529,8 @@
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="76"/>
-      <c r="B29" s="76"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="79"/>
       <c r="C29" s="8" t="s">
         <v>256</v>
       </c>
@@ -10530,8 +10548,8 @@
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="76"/>
-      <c r="B30" s="76"/>
+      <c r="A30" s="79"/>
+      <c r="B30" s="79"/>
       <c r="C30" s="8" t="s">
         <v>257</v>
       </c>
@@ -10549,10 +10567,10 @@
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="76">
+      <c r="A31" s="79">
         <v>9</v>
       </c>
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="79" t="s">
         <v>157</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -10572,8 +10590,8 @@
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="8" t="s">
         <v>259</v>
       </c>
@@ -10591,8 +10609,8 @@
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="76"/>
-      <c r="B33" s="76"/>
+      <c r="A33" s="79"/>
+      <c r="B33" s="79"/>
       <c r="C33" s="8" t="s">
         <v>260</v>
       </c>
@@ -10665,27 +10683,27 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="21">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B16:B18"/>
     <mergeCell ref="A1:M3"/>
     <mergeCell ref="F4:M4"/>
     <mergeCell ref="A6:M6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A16:A18"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10720,11 +10738,11 @@
       <c r="A4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
@@ -10750,10 +10768,10 @@
       <c r="C8" s="42">
         <v>27</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="73"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
@@ -10765,8 +10783,8 @@
       <c r="C9" s="42">
         <v>27</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
@@ -10778,8 +10796,8 @@
       <c r="C10" s="42">
         <v>27</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
@@ -10791,8 +10809,8 @@
       <c r="C11" s="42">
         <v>27</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
@@ -10804,8 +10822,8 @@
       <c r="C12" s="42">
         <v>27</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
@@ -10817,42 +10835,42 @@
       <c r="C13" s="42">
         <v>27</v>
       </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
-      <c r="I20" s="74" t="s">
+      <c r="I20" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
@@ -10893,7 +10911,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F6" sqref="F6:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10908,15 +10926,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -10951,21 +10969,21 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="59" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="55" t="s">
         <v>267</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="80" t="s">
         <v>158</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -10978,15 +10996,15 @@
         <v>198</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G6" s="26">
         <v>43389</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="78"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="34" t="s">
         <v>288</v>
       </c>
@@ -10997,17 +11015,17 @@
         <v>198</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G7" s="26">
         <v>43389</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="55" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="60" t="s">
         <v>160</v>
       </c>
       <c r="C8" s="34" t="s">
@@ -11020,15 +11038,15 @@
         <v>198</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G8" s="26">
         <v>43389</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="34" t="s">
         <v>289</v>
       </c>
@@ -11039,15 +11057,15 @@
         <v>225</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G9" s="26">
         <v>43389</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="34" t="s">
         <v>291</v>
       </c>
@@ -11058,15 +11076,15 @@
         <v>226</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G10" s="26">
         <v>43391</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="34" t="s">
         <v>292</v>
       </c>
@@ -11077,7 +11095,7 @@
         <v>227</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G11" s="26">
         <v>43391</v>
@@ -11100,17 +11118,17 @@
         <v>198</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G12" s="26">
         <v>43391</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="60" t="s">
         <v>163</v>
       </c>
       <c r="C13" s="34" t="s">
@@ -11123,15 +11141,15 @@
         <v>198</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G13" s="26">
         <v>43393</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="34" t="s">
         <v>295</v>
       </c>
@@ -11142,15 +11160,15 @@
         <v>198</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G14" s="26">
         <v>43393</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="53"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="34" t="s">
         <v>296</v>
       </c>
@@ -11161,18 +11179,18 @@
         <v>198</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G15" s="26">
         <v>43393</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="55" t="s">
         <v>273</v>
       </c>
-      <c r="B16" s="47" t="s">
-        <v>107</v>
+      <c r="B16" s="52" t="s">
+        <v>339</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>297</v>
@@ -11184,15 +11202,15 @@
         <v>225</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G16" s="26">
         <v>43394</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="34" t="s">
         <v>298</v>
       </c>
@@ -11203,15 +11221,15 @@
         <v>226</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G17" s="26">
         <v>43394</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="34" t="s">
         <v>299</v>
       </c>
@@ -11222,17 +11240,17 @@
         <v>227</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G18" s="26">
         <v>43394</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="55" t="s">
         <v>271</v>
       </c>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="83" t="s">
         <v>108</v>
       </c>
       <c r="C19" s="34" t="s">
@@ -11245,15 +11263,15 @@
         <v>225</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G19" s="26">
         <v>43395</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="53"/>
-      <c r="B20" s="80"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="83"/>
       <c r="C20" s="34" t="s">
         <v>301</v>
       </c>
@@ -11264,15 +11282,15 @@
         <v>226</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G20" s="26">
         <v>43395</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
-      <c r="B21" s="80"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="83"/>
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
@@ -11283,17 +11301,17 @@
         <v>227</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G21" s="26">
         <v>43395</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="55" t="s">
         <v>272</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="83" t="s">
         <v>111</v>
       </c>
       <c r="C22" s="34" t="s">
@@ -11306,15 +11324,15 @@
         <v>225</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G22" s="26">
         <v>43396</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="34" t="s">
         <v>304</v>
       </c>
@@ -11325,15 +11343,15 @@
         <v>226</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G23" s="26">
         <v>43396</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="53"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="34" t="s">
         <v>305</v>
       </c>
@@ -11344,7 +11362,7 @@
         <v>227</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G24" s="26">
         <v>43396</v>
@@ -11397,51 +11415,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -11459,16 +11477,16 @@
       <c r="E4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="71"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="74"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
@@ -11488,27 +11506,27 @@
       <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="77">
+      <c r="A7" s="80">
         <v>1</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="80" t="s">
         <v>158</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -11528,8 +11546,8 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="6" t="s">
         <v>275</v>
       </c>
@@ -11547,10 +11565,10 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="58">
+      <c r="A9" s="60">
         <v>2</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="60" t="s">
         <v>160</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -11570,8 +11588,8 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="6" t="s">
         <v>277</v>
       </c>
@@ -11589,8 +11607,8 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="6" t="s">
         <v>279</v>
       </c>
@@ -11608,8 +11626,8 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="6" t="s">
         <v>278</v>
       </c>
@@ -11650,10 +11668,10 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="58">
+      <c r="A14" s="60">
         <v>4</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="60" t="s">
         <v>163</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -11673,8 +11691,8 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="6" t="s">
         <v>282</v>
       </c>
@@ -11692,8 +11710,8 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="6" t="s">
         <v>283</v>
       </c>
@@ -11711,10 +11729,10 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="47">
+      <c r="A17" s="52">
         <v>5</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="52" t="s">
         <v>107</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -11734,8 +11752,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="10" t="s">
         <v>286</v>
       </c>
@@ -11753,8 +11771,8 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="43" t="s">
         <v>285</v>
       </c>
@@ -11772,10 +11790,10 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="80">
+      <c r="A20" s="83">
         <v>6</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="83" t="s">
         <v>108</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -11795,8 +11813,8 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="83"/>
       <c r="C21" s="10" t="s">
         <v>286</v>
       </c>
@@ -11814,8 +11832,8 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="44" t="s">
         <v>285</v>
       </c>
@@ -11833,10 +11851,10 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="80">
+      <c r="A23" s="83">
         <v>7</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="83" t="s">
         <v>111</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -11856,8 +11874,8 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="10" t="s">
         <v>286</v>
       </c>
@@ -11875,8 +11893,8 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
-      <c r="B25" s="80"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="83"/>
       <c r="C25" s="44" t="s">
         <v>285</v>
       </c>

</xml_diff>